<commit_message>
this is the linux version
</commit_message>
<xml_diff>
--- a/clean_datita.xlsx
+++ b/clean_datita.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2296,7 +2296,3588 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Sin datoSin dato</t>
+          <t>Sin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>02-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>16.6</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Este  5</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>02-enero-2023</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>16.6</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Este  5</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>02-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>16.6</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Este  5</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>02-enero-2023</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>16.6</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Este  5</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>03-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>23.4</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 68</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Noreste  14</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1006.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>03-enero-2023</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>23.6</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 62</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Este  14</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1006.2 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>03-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 69</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Este  20</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>03-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado con polvo levantado por viento</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>8 km</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>20.6</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 78</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Sudeste  29</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>02-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>16.6</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Este  5</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1005.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Sin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 38</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Este  7</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 38</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Este  7</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>26.2</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 38</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Este  13</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>26.2</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 38</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Este  13</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 42</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Este  16</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 42</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Noreste  16</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Este  18</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.2 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Noreste  16</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Noreste  16</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>22.8</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 44</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Norte  9</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1011.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Noreste  5</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Sin datoSin datoSin datoSin datoSin datoSin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Noreste  5</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Noreste  5</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Sin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Sin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Sin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>04-enero-2023</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>04-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Despejado</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>10 km</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>18.5</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 72</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Noreste  3</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Oeste  13</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Oeste  13</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Oeste  13</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 61</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Oeste  13</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>21.8</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 52</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Noroeste  9</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1015 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>21.8</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 52</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Noroeste  9</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1015 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>21.8</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 52</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Noroeste  9</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1015 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>21.8</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 52</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Noroeste  9</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1015 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Norte  11</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Norte  11</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Norte  11</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Norte  11</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>27.1</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Noroeste  11</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>28.3</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Oeste  18</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>28.3</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Oeste  18</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 35</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Oeste  18</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1014.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>31.6</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Noroeste  11</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013.6 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>32.6</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Noroeste  13</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>05-enero-2023</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>32.6</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Noroeste  13</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Algo nublado</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>32.6</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Noroeste  13</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.8 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>33.2</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 32</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>Sudoeste  14</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.2 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>Oeste  14</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.2 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>31.8</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>32.6</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 43</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Sudeste  5</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>15 km</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>29.2</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>29.4</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Norte  9</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1012.4 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>12 km</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 58</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Noroeste  3</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Sin datoSin datoSin datoSin datoSin datoSin datoSin datoSin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>12 km</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 58</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Noroeste  3</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>12 km</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 58</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Noroeste  3</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Sin dato Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>12 km</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>22.6</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 62</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Calma</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Villa Gesell</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>05-Enero-2023</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Parcialmente nublado</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>12 km</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>22.6</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>No se calcula</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 62</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Calma</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1013 / </t>
         </is>
       </c>
     </row>

</xml_diff>